<commit_message>
this is 2nd code
</commit_message>
<xml_diff>
--- a/CLEANING SERVICE.xlsx
+++ b/CLEANING SERVICE.xlsx
@@ -657,7 +657,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -693,11 +693,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -718,16 +742,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -757,6 +775,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1077,7 +1110,7 @@
       <c r="B1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:15" ht="31.5">
       <c r="A2" s="7" t="s">
@@ -1086,7 +1119,7 @@
       <c r="B2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="7" t="s">
@@ -1095,16 +1128,16 @@
       <c r="B3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:15" ht="31.5">
       <c r="A4" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>44145</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:15" ht="31.5">
       <c r="A5" s="7" t="s">
@@ -1113,7 +1146,7 @@
       <c r="B5" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:15" ht="31.5">
       <c r="A6" s="7" t="s">
@@ -1122,39 +1155,39 @@
       <c r="B6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="17"/>
-      <c r="B7" s="10"/>
-      <c r="F7" s="18"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="9"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:15" ht="42.75">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="1"/>
@@ -1235,16 +1268,16 @@
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="30">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -1253,7 +1286,7 @@
       <c r="F11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="10" t="s">
         <v>45</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -1270,17 +1303,17 @@
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="30">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -1297,17 +1330,17 @@
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="30">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="11"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="10" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -1324,17 +1357,17 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="30">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="10" t="s">
         <v>45</v>
       </c>
       <c r="H14" s="6" t="s">
@@ -1351,17 +1384,17 @@
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" ht="30">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="9" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="8" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="10" t="s">
         <v>45</v>
       </c>
       <c r="H15" s="6" t="s">
@@ -1378,13 +1411,13 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" ht="45">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1413,9 +1446,9 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" ht="45">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="6" t="s">
         <v>58</v>
       </c>
@@ -1442,9 +1475,9 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" ht="45">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="6" t="s">
         <v>61</v>
       </c>
@@ -1471,13 +1504,13 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" ht="105">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1506,10 +1539,10 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" ht="90">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="11" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -1535,10 +1568,10 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" ht="90">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="11"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="6" t="s">
         <v>70</v>
       </c>
@@ -1597,16 +1630,16 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" ht="60">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="C23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -1632,11 +1665,11 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" ht="60">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="14" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="12" t="s">
         <v>79</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1659,11 +1692,11 @@
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:15" ht="60">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="9" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="8" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -1686,11 +1719,11 @@
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" ht="75">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="9" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="8" t="s">
         <v>81</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -1713,11 +1746,11 @@
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" ht="45">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="9" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="8" t="s">
         <v>82</v>
       </c>
       <c r="F27" s="6" t="s">
@@ -1752,7 +1785,7 @@
       <c r="D28" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F28" s="6" t="s">
@@ -1775,19 +1808,19 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:15" ht="60">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>90</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -1810,11 +1843,11 @@
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" ht="60">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="9" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="8" t="s">
         <v>91</v>
       </c>
       <c r="F30" s="6" t="s">
@@ -1837,11 +1870,11 @@
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="1:15" ht="45">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="9" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="8" t="s">
         <v>92</v>
       </c>
       <c r="F31" s="6" t="s">
@@ -1864,11 +1897,11 @@
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="1:15" ht="30">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="9" t="s">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="8" t="s">
         <v>98</v>
       </c>
       <c r="F32" s="6" t="s">
@@ -1891,11 +1924,11 @@
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:15" ht="30">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="9" t="s">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="8" t="s">
         <v>100</v>
       </c>
       <c r="F33" s="6" t="s">
@@ -1918,11 +1951,11 @@
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:15" ht="30">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="14" t="s">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="12" t="s">
         <v>93</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -1945,11 +1978,11 @@
       <c r="O34" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="60">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="9" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="8" t="s">
         <v>94</v>
       </c>
       <c r="F35" s="6" t="s">
@@ -1972,11 +2005,11 @@
       <c r="O35" s="1"/>
     </row>
     <row r="36" spans="1:15" ht="30">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="13" t="s">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="11" t="s">
         <v>105</v>
       </c>
       <c r="F36" s="6" t="s">
@@ -1998,11 +2031,11 @@
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:15" ht="45">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="13" t="s">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="11" t="s">
         <v>106</v>
       </c>
       <c r="F37" s="6" t="s">
@@ -2063,16 +2096,16 @@
       <c r="A39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="11" t="s">
+      <c r="C39" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="12" t="s">
         <v>111</v>
       </c>
       <c r="F39" s="6" t="s">
@@ -2098,10 +2131,10 @@
       <c r="A40" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="14" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="12" t="s">
         <v>113</v>
       </c>
       <c r="F40" s="6" t="s">
@@ -2127,10 +2160,10 @@
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="14" t="s">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="12" t="s">
         <v>115</v>
       </c>
       <c r="F41" s="6" t="s">
@@ -2150,10 +2183,10 @@
       <c r="A42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="14" t="s">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="12" t="s">
         <v>117</v>
       </c>
       <c r="F42" s="6" t="s">
@@ -2170,16 +2203,16 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="45">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="11" t="s">
+      <c r="C43" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>129</v>
       </c>
       <c r="E43" s="6" t="s">
@@ -2199,11 +2232,11 @@
       </c>
     </row>
     <row r="44" spans="1:15" ht="45">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="13" t="s">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="11" t="s">
         <v>119</v>
       </c>
       <c r="F44" s="6" t="s">
@@ -2220,11 +2253,11 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="60">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="13" t="s">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="11" t="s">
         <v>125</v>
       </c>
       <c r="F45" s="6" t="s">
@@ -2241,11 +2274,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="60">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="13" t="s">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="11" t="s">
         <v>120</v>
       </c>
       <c r="F46" s="6" t="s">
@@ -2262,11 +2295,11 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="75">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="13" t="s">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="11" t="s">
         <v>121</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -2283,11 +2316,11 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="90">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="13" t="s">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="11" t="s">
         <v>122</v>
       </c>
       <c r="F48" s="6" t="s">
@@ -2307,13 +2340,13 @@
       <c r="A49" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="11" t="s">
+      <c r="C49" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="21" t="s">
         <v>138</v>
       </c>
       <c r="E49" s="6" t="s">
@@ -2336,10 +2369,10 @@
       <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="15" t="s">
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="13" t="s">
         <v>135</v>
       </c>
       <c r="F50" s="6" t="s">
@@ -2359,10 +2392,10 @@
       <c r="A51" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="15" t="s">
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="13" t="s">
         <v>130</v>
       </c>
       <c r="F51" s="6" t="s">
@@ -2378,14 +2411,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="75">
+    <row r="52" spans="1:9" ht="60">
       <c r="A52" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="15" t="s">
+      <c r="B52" s="20"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="13" t="s">
         <v>131</v>
       </c>
       <c r="F52" s="6" t="s">
@@ -2405,10 +2438,10 @@
       <c r="A53" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="15" t="s">
+      <c r="B53" s="20"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F53" s="6" t="s">
@@ -2454,16 +2487,16 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="45">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="11" t="s">
+      <c r="C55" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>141</v>
       </c>
       <c r="E55" s="4" t="s">
@@ -2483,10 +2516,10 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="45">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
       <c r="E56" s="4" t="s">
         <v>144</v>
       </c>
@@ -2504,10 +2537,10 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="45">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
       <c r="E57" s="4" t="s">
         <v>146</v>
       </c>
@@ -2525,10 +2558,10 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="30">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="4" t="s">
         <v>148</v>
       </c>
@@ -2546,10 +2579,10 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="30">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="4" t="s">
         <v>150</v>
       </c>
@@ -2567,16 +2600,16 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="48" customHeight="1">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" s="8" t="s">
+      <c r="C60" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>153</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -2596,65 +2629,65 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="118.5" customHeight="1">
-      <c r="A61" s="3"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
       <c r="E61" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="16" t="s">
+      <c r="F61" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="H61" s="16" t="s">
+      <c r="H61" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="I61" s="16" t="s">
+      <c r="I61" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="75">
-      <c r="A62" s="3"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
       <c r="E62" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F62" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I62" s="16" t="s">
+      <c r="F62" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I62" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="30">
-      <c r="A63" s="3"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
       <c r="E63" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F63" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="16" t="s">
+      <c r="F63" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="H63" s="16" t="s">
+      <c r="H63" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="I63" s="16" t="s">
+      <c r="I63" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2893,31 +2926,33 @@
       <c r="F141"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="37">
+    <mergeCell ref="D55:D59"/>
+    <mergeCell ref="C55:C59"/>
     <mergeCell ref="B55:B59"/>
     <mergeCell ref="A55:A59"/>
     <mergeCell ref="D60:D63"/>
     <mergeCell ref="C60:C63"/>
     <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="B43:B48"/>
     <mergeCell ref="D49:D53"/>
     <mergeCell ref="C49:C53"/>
     <mergeCell ref="B49:B53"/>
-    <mergeCell ref="D55:D59"/>
-    <mergeCell ref="C55:C59"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
     <mergeCell ref="D29:D37"/>
     <mergeCell ref="C29:C37"/>
     <mergeCell ref="B29:B37"/>
     <mergeCell ref="A29:A37"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="A16:A18"/>
@@ -2925,11 +2960,10 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>